<commit_message>
Make the file more generic
</commit_message>
<xml_diff>
--- a/data-export_commands-builder.xlsx
+++ b/data-export_commands-builder.xlsx
@@ -1,30 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CurDev\_Github-pthivierge\data-reader-cmdline\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CurDev\.github pthivierge\data-reader-cmdline\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49F49FAB-3B3F-4CC8-97F3-FF1A84ACF59D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14520"/>
+    <workbookView xWindow="9960" yWindow="630" windowWidth="29430" windowHeight="19995" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Command</t>
   </si>
@@ -53,21 +63,12 @@
     <t>eventsPerFile</t>
   </si>
   <si>
-    <t>WYCWAPPH059</t>
-  </si>
-  <si>
     <t>Unit</t>
   </si>
   <si>
     <t>StarTtime</t>
   </si>
   <si>
-    <t xml:space="preserve"> 23/07/2013 02:14:03</t>
-  </si>
-  <si>
-    <t>16/05/2015 09:04:47</t>
-  </si>
-  <si>
     <t>estimatedTagsCount</t>
   </si>
   <si>
@@ -105,12 +106,18 @@
   </si>
   <si>
     <t>Many celles in this workbook contains formulas, be careful to not overwrite them.</t>
+  </si>
+  <si>
+    <t>PIDA01</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy/mm/dd\ hh:mm:ss"/>
+  </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -227,7 +234,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -241,6 +248,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="2" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Input" xfId="1" builtinId="20"/>
@@ -522,35 +532,35 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:D43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.7109375" customWidth="1"/>
     <col min="2" max="2" width="25.28515625" customWidth="1"/>
-    <col min="3" max="3" width="73.85546875" customWidth="1"/>
+    <col min="3" max="3" width="33.28515625" customWidth="1"/>
     <col min="4" max="4" width="255.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="6"/>
       <c r="B1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="8"/>
       <c r="B2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -558,32 +568,32 @@
         <v>1</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
+      </c>
+      <c r="B6" s="9">
+        <v>42005</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>13</v>
+      <c r="B7" s="9">
+        <v>43831</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -594,7 +604,7 @@
         <v>1</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -605,7 +615,7 @@
         <v>100000</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -616,7 +626,7 @@
         <v>8</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -627,28 +637,28 @@
         <v>100000001</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B12" s="5">
         <v>100000</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D15" s="8" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>2</v>
@@ -665,16 +675,16 @@
         <v>1000</v>
       </c>
       <c r="B17" s="2" t="str">
-        <f>CONCATENATE("Unity",A17,"*.Value",)</f>
-        <v>Unity1000*.Value</v>
+        <f>CONCATENATE("Unit",A17,"*.Value",)</f>
+        <v>Unit1000*.Value</v>
       </c>
       <c r="C17" t="str">
-        <f>CONCATENATE("\\WYCVWAPPH186\D$\Stage\MDUS_Export\Reads\Extract_PH3_",A17,"_")</f>
-        <v>\\WYCVWAPPH186\D$\Stage\MDUS_Export\Reads\Extract_PH3_1000_</v>
+        <f>CONCATENATE("C:\exported-data\",A17,"_")</f>
+        <v>C:\exported-data\1000_</v>
       </c>
       <c r="D17" t="str">
-        <f>"DataReader.exe -s " &amp; $B$5  &amp; " -t """ &amp; B17 &amp; """ --st """&amp;$B$6&amp;""" --et """ &amp; $B$7&amp; """ --estimatedEventsPerDay " &amp; $B$8 &amp; " --eventsPerRead " &amp; $B$9 &amp;" --eventsPerFile " &amp; $B$11 &amp;" --estimatedTagscount " &amp; $B$12 &amp;" --writersCount " &amp; $B$10 &amp;" --enableWrite --outFileName """ &amp;C17 &amp;""""</f>
-        <v>DataReader.exe -s WYCWAPPH059 -t "Unity1000*.Value" --st " 23/07/2013 02:14:03" --et "16/05/2015 09:04:47" --estimatedEventsPerDay 1 --eventsPerRead 100000 --eventsPerFile 100000001 --estimatedTagscount 100000 --writersCount 8 --enableWrite --outFileName "\\WYCVWAPPH186\D$\Stage\MDUS_Export\Reads\Extract_PH3_1000_"</v>
+        <f>"DataReader.exe -s " &amp; $B$5  &amp; " -t """ &amp; B17 &amp; """ --st """ &amp; TEXT($B$6,"YYYY-MM-dd HH:mm:ss") &amp; """ --et """ &amp; TEXT($B$7,"YYYY-MM-dd HH:mm:ss") &amp; """ --estimatedEventsPerDay " &amp; $B$8 &amp; " --eventsPerRead " &amp; $B$9 &amp;" --eventsPerFile " &amp; $B$11 &amp;" --estimatedTagscount " &amp; $B$12 &amp;" --writersCount " &amp; $B$10 &amp;" --enableWrite --outFileName """ &amp;C17 &amp;""""</f>
+        <v>DataReader.exe -s PIDA01 -t "Unit1000*.Value" --st "2015-01-01 00:00:00" --et "2020-01-01 00:00:00" --estimatedEventsPerDay 1 --eventsPerRead 100000 --eventsPerFile 100000001 --estimatedTagscount 100000 --writersCount 8 --enableWrite --outFileName "C:\exported-data\1000_"</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -682,16 +692,16 @@
         <v>1001</v>
       </c>
       <c r="B18" s="2" t="str">
-        <f t="shared" ref="B18:B43" si="0">CONCATENATE("Unity",A18,"*.Value",)</f>
-        <v>Unity1001*.Value</v>
+        <f t="shared" ref="B18:B43" si="0">CONCATENATE("Unit",A18,"*.Value",)</f>
+        <v>Unit1001*.Value</v>
       </c>
       <c r="C18" t="str">
-        <f t="shared" ref="C18:C43" si="1">CONCATENATE("\\WYCVWAPPH186\D$\Stage\MDUS_Export\Reads\Extract_PH3_",A18,"_")</f>
-        <v>\\WYCVWAPPH186\D$\Stage\MDUS_Export\Reads\Extract_PH3_1001_</v>
+        <f t="shared" ref="C18:C43" si="1">CONCATENATE("C:\exported-data\",A18,"_")</f>
+        <v>C:\exported-data\1001_</v>
       </c>
       <c r="D18" t="str">
-        <f t="shared" ref="D18:D43" si="2">"DataReader.exe -s " &amp; $B$5  &amp; " -t """ &amp; B18 &amp; """ --st """&amp;$B$6&amp;""" --et """ &amp; $B$7&amp; """ --estimatedEventsPerDay " &amp; $B$8 &amp; " --eventsPerRead " &amp; $B$9 &amp;" --eventsPerFile " &amp; $B$11 &amp;" --estimatedTagscount " &amp; $B$12 &amp;" --writersCount " &amp; $B$10 &amp;" --enableWrite --outFileName """ &amp;C18 &amp;""""</f>
-        <v>DataReader.exe -s WYCWAPPH059 -t "Unity1001*.Value" --st " 23/07/2013 02:14:03" --et "16/05/2015 09:04:47" --estimatedEventsPerDay 1 --eventsPerRead 100000 --eventsPerFile 100000001 --estimatedTagscount 100000 --writersCount 8 --enableWrite --outFileName "\\WYCVWAPPH186\D$\Stage\MDUS_Export\Reads\Extract_PH3_1001_"</v>
+        <f t="shared" ref="D18:D43" si="2">"DataReader.exe -s " &amp; $B$5  &amp; " -t """ &amp; B18 &amp; """ --st """ &amp; TEXT($B$6,"YYYY-MM-dd HH:mm:ss") &amp; """ --et """ &amp; TEXT($B$7,"YYYY-MM-dd HH:mm:ss") &amp; """ --estimatedEventsPerDay " &amp; $B$8 &amp; " --eventsPerRead " &amp; $B$9 &amp;" --eventsPerFile " &amp; $B$11 &amp;" --estimatedTagscount " &amp; $B$12 &amp;" --writersCount " &amp; $B$10 &amp;" --enableWrite --outFileName """ &amp;C18 &amp;""""</f>
+        <v>DataReader.exe -s PIDA01 -t "Unit1001*.Value" --st "2015-01-01 00:00:00" --et "2020-01-01 00:00:00" --estimatedEventsPerDay 1 --eventsPerRead 100000 --eventsPerFile 100000001 --estimatedTagscount 100000 --writersCount 8 --enableWrite --outFileName "C:\exported-data\1001_"</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -700,15 +710,15 @@
       </c>
       <c r="B19" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>Unity1002*.Value</v>
+        <v>Unit1002*.Value</v>
       </c>
       <c r="C19" t="str">
         <f t="shared" si="1"/>
-        <v>\\WYCVWAPPH186\D$\Stage\MDUS_Export\Reads\Extract_PH3_1002_</v>
+        <v>C:\exported-data\1002_</v>
       </c>
       <c r="D19" t="str">
         <f t="shared" si="2"/>
-        <v>DataReader.exe -s WYCWAPPH059 -t "Unity1002*.Value" --st " 23/07/2013 02:14:03" --et "16/05/2015 09:04:47" --estimatedEventsPerDay 1 --eventsPerRead 100000 --eventsPerFile 100000001 --estimatedTagscount 100000 --writersCount 8 --enableWrite --outFileName "\\WYCVWAPPH186\D$\Stage\MDUS_Export\Reads\Extract_PH3_1002_"</v>
+        <v>DataReader.exe -s PIDA01 -t "Unit1002*.Value" --st "2015-01-01 00:00:00" --et "2020-01-01 00:00:00" --estimatedEventsPerDay 1 --eventsPerRead 100000 --eventsPerFile 100000001 --estimatedTagscount 100000 --writersCount 8 --enableWrite --outFileName "C:\exported-data\1002_"</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -717,15 +727,15 @@
       </c>
       <c r="B20" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>Unity1003*.Value</v>
+        <v>Unit1003*.Value</v>
       </c>
       <c r="C20" t="str">
         <f t="shared" si="1"/>
-        <v>\\WYCVWAPPH186\D$\Stage\MDUS_Export\Reads\Extract_PH3_1003_</v>
+        <v>C:\exported-data\1003_</v>
       </c>
       <c r="D20" t="str">
         <f t="shared" si="2"/>
-        <v>DataReader.exe -s WYCWAPPH059 -t "Unity1003*.Value" --st " 23/07/2013 02:14:03" --et "16/05/2015 09:04:47" --estimatedEventsPerDay 1 --eventsPerRead 100000 --eventsPerFile 100000001 --estimatedTagscount 100000 --writersCount 8 --enableWrite --outFileName "\\WYCVWAPPH186\D$\Stage\MDUS_Export\Reads\Extract_PH3_1003_"</v>
+        <v>DataReader.exe -s PIDA01 -t "Unit1003*.Value" --st "2015-01-01 00:00:00" --et "2020-01-01 00:00:00" --estimatedEventsPerDay 1 --eventsPerRead 100000 --eventsPerFile 100000001 --estimatedTagscount 100000 --writersCount 8 --enableWrite --outFileName "C:\exported-data\1003_"</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -734,15 +744,15 @@
       </c>
       <c r="B21" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>Unity1004*.Value</v>
+        <v>Unit1004*.Value</v>
       </c>
       <c r="C21" t="str">
         <f t="shared" si="1"/>
-        <v>\\WYCVWAPPH186\D$\Stage\MDUS_Export\Reads\Extract_PH3_1004_</v>
+        <v>C:\exported-data\1004_</v>
       </c>
       <c r="D21" t="str">
         <f t="shared" si="2"/>
-        <v>DataReader.exe -s WYCWAPPH059 -t "Unity1004*.Value" --st " 23/07/2013 02:14:03" --et "16/05/2015 09:04:47" --estimatedEventsPerDay 1 --eventsPerRead 100000 --eventsPerFile 100000001 --estimatedTagscount 100000 --writersCount 8 --enableWrite --outFileName "\\WYCVWAPPH186\D$\Stage\MDUS_Export\Reads\Extract_PH3_1004_"</v>
+        <v>DataReader.exe -s PIDA01 -t "Unit1004*.Value" --st "2015-01-01 00:00:00" --et "2020-01-01 00:00:00" --estimatedEventsPerDay 1 --eventsPerRead 100000 --eventsPerFile 100000001 --estimatedTagscount 100000 --writersCount 8 --enableWrite --outFileName "C:\exported-data\1004_"</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -751,15 +761,15 @@
       </c>
       <c r="B22" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>Unity1005*.Value</v>
+        <v>Unit1005*.Value</v>
       </c>
       <c r="C22" t="str">
         <f t="shared" si="1"/>
-        <v>\\WYCVWAPPH186\D$\Stage\MDUS_Export\Reads\Extract_PH3_1005_</v>
+        <v>C:\exported-data\1005_</v>
       </c>
       <c r="D22" t="str">
         <f t="shared" si="2"/>
-        <v>DataReader.exe -s WYCWAPPH059 -t "Unity1005*.Value" --st " 23/07/2013 02:14:03" --et "16/05/2015 09:04:47" --estimatedEventsPerDay 1 --eventsPerRead 100000 --eventsPerFile 100000001 --estimatedTagscount 100000 --writersCount 8 --enableWrite --outFileName "\\WYCVWAPPH186\D$\Stage\MDUS_Export\Reads\Extract_PH3_1005_"</v>
+        <v>DataReader.exe -s PIDA01 -t "Unit1005*.Value" --st "2015-01-01 00:00:00" --et "2020-01-01 00:00:00" --estimatedEventsPerDay 1 --eventsPerRead 100000 --eventsPerFile 100000001 --estimatedTagscount 100000 --writersCount 8 --enableWrite --outFileName "C:\exported-data\1005_"</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -768,15 +778,15 @@
       </c>
       <c r="B23" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>Unity1006*.Value</v>
+        <v>Unit1006*.Value</v>
       </c>
       <c r="C23" t="str">
         <f t="shared" si="1"/>
-        <v>\\WYCVWAPPH186\D$\Stage\MDUS_Export\Reads\Extract_PH3_1006_</v>
+        <v>C:\exported-data\1006_</v>
       </c>
       <c r="D23" t="str">
         <f t="shared" si="2"/>
-        <v>DataReader.exe -s WYCWAPPH059 -t "Unity1006*.Value" --st " 23/07/2013 02:14:03" --et "16/05/2015 09:04:47" --estimatedEventsPerDay 1 --eventsPerRead 100000 --eventsPerFile 100000001 --estimatedTagscount 100000 --writersCount 8 --enableWrite --outFileName "\\WYCVWAPPH186\D$\Stage\MDUS_Export\Reads\Extract_PH3_1006_"</v>
+        <v>DataReader.exe -s PIDA01 -t "Unit1006*.Value" --st "2015-01-01 00:00:00" --et "2020-01-01 00:00:00" --estimatedEventsPerDay 1 --eventsPerRead 100000 --eventsPerFile 100000001 --estimatedTagscount 100000 --writersCount 8 --enableWrite --outFileName "C:\exported-data\1006_"</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -785,15 +795,15 @@
       </c>
       <c r="B24" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>Unity1007*.Value</v>
+        <v>Unit1007*.Value</v>
       </c>
       <c r="C24" t="str">
         <f t="shared" si="1"/>
-        <v>\\WYCVWAPPH186\D$\Stage\MDUS_Export\Reads\Extract_PH3_1007_</v>
+        <v>C:\exported-data\1007_</v>
       </c>
       <c r="D24" t="str">
         <f t="shared" si="2"/>
-        <v>DataReader.exe -s WYCWAPPH059 -t "Unity1007*.Value" --st " 23/07/2013 02:14:03" --et "16/05/2015 09:04:47" --estimatedEventsPerDay 1 --eventsPerRead 100000 --eventsPerFile 100000001 --estimatedTagscount 100000 --writersCount 8 --enableWrite --outFileName "\\WYCVWAPPH186\D$\Stage\MDUS_Export\Reads\Extract_PH3_1007_"</v>
+        <v>DataReader.exe -s PIDA01 -t "Unit1007*.Value" --st "2015-01-01 00:00:00" --et "2020-01-01 00:00:00" --estimatedEventsPerDay 1 --eventsPerRead 100000 --eventsPerFile 100000001 --estimatedTagscount 100000 --writersCount 8 --enableWrite --outFileName "C:\exported-data\1007_"</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -802,15 +812,15 @@
       </c>
       <c r="B25" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>Unity1008*.Value</v>
+        <v>Unit1008*.Value</v>
       </c>
       <c r="C25" t="str">
         <f t="shared" si="1"/>
-        <v>\\WYCVWAPPH186\D$\Stage\MDUS_Export\Reads\Extract_PH3_1008_</v>
+        <v>C:\exported-data\1008_</v>
       </c>
       <c r="D25" t="str">
         <f t="shared" si="2"/>
-        <v>DataReader.exe -s WYCWAPPH059 -t "Unity1008*.Value" --st " 23/07/2013 02:14:03" --et "16/05/2015 09:04:47" --estimatedEventsPerDay 1 --eventsPerRead 100000 --eventsPerFile 100000001 --estimatedTagscount 100000 --writersCount 8 --enableWrite --outFileName "\\WYCVWAPPH186\D$\Stage\MDUS_Export\Reads\Extract_PH3_1008_"</v>
+        <v>DataReader.exe -s PIDA01 -t "Unit1008*.Value" --st "2015-01-01 00:00:00" --et "2020-01-01 00:00:00" --estimatedEventsPerDay 1 --eventsPerRead 100000 --eventsPerFile 100000001 --estimatedTagscount 100000 --writersCount 8 --enableWrite --outFileName "C:\exported-data\1008_"</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -819,15 +829,15 @@
       </c>
       <c r="B26" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>Unity1009*.Value</v>
+        <v>Unit1009*.Value</v>
       </c>
       <c r="C26" t="str">
         <f t="shared" si="1"/>
-        <v>\\WYCVWAPPH186\D$\Stage\MDUS_Export\Reads\Extract_PH3_1009_</v>
+        <v>C:\exported-data\1009_</v>
       </c>
       <c r="D26" t="str">
         <f t="shared" si="2"/>
-        <v>DataReader.exe -s WYCWAPPH059 -t "Unity1009*.Value" --st " 23/07/2013 02:14:03" --et "16/05/2015 09:04:47" --estimatedEventsPerDay 1 --eventsPerRead 100000 --eventsPerFile 100000001 --estimatedTagscount 100000 --writersCount 8 --enableWrite --outFileName "\\WYCVWAPPH186\D$\Stage\MDUS_Export\Reads\Extract_PH3_1009_"</v>
+        <v>DataReader.exe -s PIDA01 -t "Unit1009*.Value" --st "2015-01-01 00:00:00" --et "2020-01-01 00:00:00" --estimatedEventsPerDay 1 --eventsPerRead 100000 --eventsPerFile 100000001 --estimatedTagscount 100000 --writersCount 8 --enableWrite --outFileName "C:\exported-data\1009_"</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -836,15 +846,15 @@
       </c>
       <c r="B27" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>Unity1010*.Value</v>
+        <v>Unit1010*.Value</v>
       </c>
       <c r="C27" t="str">
         <f t="shared" si="1"/>
-        <v>\\WYCVWAPPH186\D$\Stage\MDUS_Export\Reads\Extract_PH3_1010_</v>
+        <v>C:\exported-data\1010_</v>
       </c>
       <c r="D27" t="str">
         <f t="shared" si="2"/>
-        <v>DataReader.exe -s WYCWAPPH059 -t "Unity1010*.Value" --st " 23/07/2013 02:14:03" --et "16/05/2015 09:04:47" --estimatedEventsPerDay 1 --eventsPerRead 100000 --eventsPerFile 100000001 --estimatedTagscount 100000 --writersCount 8 --enableWrite --outFileName "\\WYCVWAPPH186\D$\Stage\MDUS_Export\Reads\Extract_PH3_1010_"</v>
+        <v>DataReader.exe -s PIDA01 -t "Unit1010*.Value" --st "2015-01-01 00:00:00" --et "2020-01-01 00:00:00" --estimatedEventsPerDay 1 --eventsPerRead 100000 --eventsPerFile 100000001 --estimatedTagscount 100000 --writersCount 8 --enableWrite --outFileName "C:\exported-data\1010_"</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -853,15 +863,15 @@
       </c>
       <c r="B28" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>Unity1011*.Value</v>
+        <v>Unit1011*.Value</v>
       </c>
       <c r="C28" t="str">
         <f t="shared" si="1"/>
-        <v>\\WYCVWAPPH186\D$\Stage\MDUS_Export\Reads\Extract_PH3_1011_</v>
+        <v>C:\exported-data\1011_</v>
       </c>
       <c r="D28" t="str">
         <f t="shared" si="2"/>
-        <v>DataReader.exe -s WYCWAPPH059 -t "Unity1011*.Value" --st " 23/07/2013 02:14:03" --et "16/05/2015 09:04:47" --estimatedEventsPerDay 1 --eventsPerRead 100000 --eventsPerFile 100000001 --estimatedTagscount 100000 --writersCount 8 --enableWrite --outFileName "\\WYCVWAPPH186\D$\Stage\MDUS_Export\Reads\Extract_PH3_1011_"</v>
+        <v>DataReader.exe -s PIDA01 -t "Unit1011*.Value" --st "2015-01-01 00:00:00" --et "2020-01-01 00:00:00" --estimatedEventsPerDay 1 --eventsPerRead 100000 --eventsPerFile 100000001 --estimatedTagscount 100000 --writersCount 8 --enableWrite --outFileName "C:\exported-data\1011_"</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -870,15 +880,15 @@
       </c>
       <c r="B29" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>Unity1012*.Value</v>
+        <v>Unit1012*.Value</v>
       </c>
       <c r="C29" t="str">
         <f t="shared" si="1"/>
-        <v>\\WYCVWAPPH186\D$\Stage\MDUS_Export\Reads\Extract_PH3_1012_</v>
+        <v>C:\exported-data\1012_</v>
       </c>
       <c r="D29" t="str">
         <f t="shared" si="2"/>
-        <v>DataReader.exe -s WYCWAPPH059 -t "Unity1012*.Value" --st " 23/07/2013 02:14:03" --et "16/05/2015 09:04:47" --estimatedEventsPerDay 1 --eventsPerRead 100000 --eventsPerFile 100000001 --estimatedTagscount 100000 --writersCount 8 --enableWrite --outFileName "\\WYCVWAPPH186\D$\Stage\MDUS_Export\Reads\Extract_PH3_1012_"</v>
+        <v>DataReader.exe -s PIDA01 -t "Unit1012*.Value" --st "2015-01-01 00:00:00" --et "2020-01-01 00:00:00" --estimatedEventsPerDay 1 --eventsPerRead 100000 --eventsPerFile 100000001 --estimatedTagscount 100000 --writersCount 8 --enableWrite --outFileName "C:\exported-data\1012_"</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -887,15 +897,15 @@
       </c>
       <c r="B30" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>Unity1013*.Value</v>
+        <v>Unit1013*.Value</v>
       </c>
       <c r="C30" t="str">
         <f t="shared" si="1"/>
-        <v>\\WYCVWAPPH186\D$\Stage\MDUS_Export\Reads\Extract_PH3_1013_</v>
+        <v>C:\exported-data\1013_</v>
       </c>
       <c r="D30" t="str">
         <f t="shared" si="2"/>
-        <v>DataReader.exe -s WYCWAPPH059 -t "Unity1013*.Value" --st " 23/07/2013 02:14:03" --et "16/05/2015 09:04:47" --estimatedEventsPerDay 1 --eventsPerRead 100000 --eventsPerFile 100000001 --estimatedTagscount 100000 --writersCount 8 --enableWrite --outFileName "\\WYCVWAPPH186\D$\Stage\MDUS_Export\Reads\Extract_PH3_1013_"</v>
+        <v>DataReader.exe -s PIDA01 -t "Unit1013*.Value" --st "2015-01-01 00:00:00" --et "2020-01-01 00:00:00" --estimatedEventsPerDay 1 --eventsPerRead 100000 --eventsPerFile 100000001 --estimatedTagscount 100000 --writersCount 8 --enableWrite --outFileName "C:\exported-data\1013_"</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -904,15 +914,15 @@
       </c>
       <c r="B31" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>Unity1014*.Value</v>
+        <v>Unit1014*.Value</v>
       </c>
       <c r="C31" t="str">
         <f t="shared" si="1"/>
-        <v>\\WYCVWAPPH186\D$\Stage\MDUS_Export\Reads\Extract_PH3_1014_</v>
+        <v>C:\exported-data\1014_</v>
       </c>
       <c r="D31" t="str">
         <f t="shared" si="2"/>
-        <v>DataReader.exe -s WYCWAPPH059 -t "Unity1014*.Value" --st " 23/07/2013 02:14:03" --et "16/05/2015 09:04:47" --estimatedEventsPerDay 1 --eventsPerRead 100000 --eventsPerFile 100000001 --estimatedTagscount 100000 --writersCount 8 --enableWrite --outFileName "\\WYCVWAPPH186\D$\Stage\MDUS_Export\Reads\Extract_PH3_1014_"</v>
+        <v>DataReader.exe -s PIDA01 -t "Unit1014*.Value" --st "2015-01-01 00:00:00" --et "2020-01-01 00:00:00" --estimatedEventsPerDay 1 --eventsPerRead 100000 --eventsPerFile 100000001 --estimatedTagscount 100000 --writersCount 8 --enableWrite --outFileName "C:\exported-data\1014_"</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -921,15 +931,15 @@
       </c>
       <c r="B32" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>Unity1015*.Value</v>
+        <v>Unit1015*.Value</v>
       </c>
       <c r="C32" t="str">
         <f t="shared" si="1"/>
-        <v>\\WYCVWAPPH186\D$\Stage\MDUS_Export\Reads\Extract_PH3_1015_</v>
+        <v>C:\exported-data\1015_</v>
       </c>
       <c r="D32" t="str">
         <f t="shared" si="2"/>
-        <v>DataReader.exe -s WYCWAPPH059 -t "Unity1015*.Value" --st " 23/07/2013 02:14:03" --et "16/05/2015 09:04:47" --estimatedEventsPerDay 1 --eventsPerRead 100000 --eventsPerFile 100000001 --estimatedTagscount 100000 --writersCount 8 --enableWrite --outFileName "\\WYCVWAPPH186\D$\Stage\MDUS_Export\Reads\Extract_PH3_1015_"</v>
+        <v>DataReader.exe -s PIDA01 -t "Unit1015*.Value" --st "2015-01-01 00:00:00" --et "2020-01-01 00:00:00" --estimatedEventsPerDay 1 --eventsPerRead 100000 --eventsPerFile 100000001 --estimatedTagscount 100000 --writersCount 8 --enableWrite --outFileName "C:\exported-data\1015_"</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -938,15 +948,15 @@
       </c>
       <c r="B33" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>Unity1016*.Value</v>
+        <v>Unit1016*.Value</v>
       </c>
       <c r="C33" t="str">
         <f t="shared" si="1"/>
-        <v>\\WYCVWAPPH186\D$\Stage\MDUS_Export\Reads\Extract_PH3_1016_</v>
+        <v>C:\exported-data\1016_</v>
       </c>
       <c r="D33" t="str">
         <f t="shared" si="2"/>
-        <v>DataReader.exe -s WYCWAPPH059 -t "Unity1016*.Value" --st " 23/07/2013 02:14:03" --et "16/05/2015 09:04:47" --estimatedEventsPerDay 1 --eventsPerRead 100000 --eventsPerFile 100000001 --estimatedTagscount 100000 --writersCount 8 --enableWrite --outFileName "\\WYCVWAPPH186\D$\Stage\MDUS_Export\Reads\Extract_PH3_1016_"</v>
+        <v>DataReader.exe -s PIDA01 -t "Unit1016*.Value" --st "2015-01-01 00:00:00" --et "2020-01-01 00:00:00" --estimatedEventsPerDay 1 --eventsPerRead 100000 --eventsPerFile 100000001 --estimatedTagscount 100000 --writersCount 8 --enableWrite --outFileName "C:\exported-data\1016_"</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -955,15 +965,15 @@
       </c>
       <c r="B34" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>Unity1017*.Value</v>
+        <v>Unit1017*.Value</v>
       </c>
       <c r="C34" t="str">
         <f t="shared" si="1"/>
-        <v>\\WYCVWAPPH186\D$\Stage\MDUS_Export\Reads\Extract_PH3_1017_</v>
+        <v>C:\exported-data\1017_</v>
       </c>
       <c r="D34" t="str">
         <f t="shared" si="2"/>
-        <v>DataReader.exe -s WYCWAPPH059 -t "Unity1017*.Value" --st " 23/07/2013 02:14:03" --et "16/05/2015 09:04:47" --estimatedEventsPerDay 1 --eventsPerRead 100000 --eventsPerFile 100000001 --estimatedTagscount 100000 --writersCount 8 --enableWrite --outFileName "\\WYCVWAPPH186\D$\Stage\MDUS_Export\Reads\Extract_PH3_1017_"</v>
+        <v>DataReader.exe -s PIDA01 -t "Unit1017*.Value" --st "2015-01-01 00:00:00" --et "2020-01-01 00:00:00" --estimatedEventsPerDay 1 --eventsPerRead 100000 --eventsPerFile 100000001 --estimatedTagscount 100000 --writersCount 8 --enableWrite --outFileName "C:\exported-data\1017_"</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -972,15 +982,15 @@
       </c>
       <c r="B35" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>Unity1018*.Value</v>
+        <v>Unit1018*.Value</v>
       </c>
       <c r="C35" t="str">
         <f t="shared" si="1"/>
-        <v>\\WYCVWAPPH186\D$\Stage\MDUS_Export\Reads\Extract_PH3_1018_</v>
+        <v>C:\exported-data\1018_</v>
       </c>
       <c r="D35" t="str">
         <f t="shared" si="2"/>
-        <v>DataReader.exe -s WYCWAPPH059 -t "Unity1018*.Value" --st " 23/07/2013 02:14:03" --et "16/05/2015 09:04:47" --estimatedEventsPerDay 1 --eventsPerRead 100000 --eventsPerFile 100000001 --estimatedTagscount 100000 --writersCount 8 --enableWrite --outFileName "\\WYCVWAPPH186\D$\Stage\MDUS_Export\Reads\Extract_PH3_1018_"</v>
+        <v>DataReader.exe -s PIDA01 -t "Unit1018*.Value" --st "2015-01-01 00:00:00" --et "2020-01-01 00:00:00" --estimatedEventsPerDay 1 --eventsPerRead 100000 --eventsPerFile 100000001 --estimatedTagscount 100000 --writersCount 8 --enableWrite --outFileName "C:\exported-data\1018_"</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -989,15 +999,15 @@
       </c>
       <c r="B36" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>Unity1019*.Value</v>
+        <v>Unit1019*.Value</v>
       </c>
       <c r="C36" t="str">
         <f t="shared" si="1"/>
-        <v>\\WYCVWAPPH186\D$\Stage\MDUS_Export\Reads\Extract_PH3_1019_</v>
+        <v>C:\exported-data\1019_</v>
       </c>
       <c r="D36" t="str">
         <f t="shared" si="2"/>
-        <v>DataReader.exe -s WYCWAPPH059 -t "Unity1019*.Value" --st " 23/07/2013 02:14:03" --et "16/05/2015 09:04:47" --estimatedEventsPerDay 1 --eventsPerRead 100000 --eventsPerFile 100000001 --estimatedTagscount 100000 --writersCount 8 --enableWrite --outFileName "\\WYCVWAPPH186\D$\Stage\MDUS_Export\Reads\Extract_PH3_1019_"</v>
+        <v>DataReader.exe -s PIDA01 -t "Unit1019*.Value" --st "2015-01-01 00:00:00" --et "2020-01-01 00:00:00" --estimatedEventsPerDay 1 --eventsPerRead 100000 --eventsPerFile 100000001 --estimatedTagscount 100000 --writersCount 8 --enableWrite --outFileName "C:\exported-data\1019_"</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -1006,15 +1016,15 @@
       </c>
       <c r="B37" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>Unity1020*.Value</v>
+        <v>Unit1020*.Value</v>
       </c>
       <c r="C37" t="str">
         <f t="shared" si="1"/>
-        <v>\\WYCVWAPPH186\D$\Stage\MDUS_Export\Reads\Extract_PH3_1020_</v>
+        <v>C:\exported-data\1020_</v>
       </c>
       <c r="D37" t="str">
         <f t="shared" si="2"/>
-        <v>DataReader.exe -s WYCWAPPH059 -t "Unity1020*.Value" --st " 23/07/2013 02:14:03" --et "16/05/2015 09:04:47" --estimatedEventsPerDay 1 --eventsPerRead 100000 --eventsPerFile 100000001 --estimatedTagscount 100000 --writersCount 8 --enableWrite --outFileName "\\WYCVWAPPH186\D$\Stage\MDUS_Export\Reads\Extract_PH3_1020_"</v>
+        <v>DataReader.exe -s PIDA01 -t "Unit1020*.Value" --st "2015-01-01 00:00:00" --et "2020-01-01 00:00:00" --estimatedEventsPerDay 1 --eventsPerRead 100000 --eventsPerFile 100000001 --estimatedTagscount 100000 --writersCount 8 --enableWrite --outFileName "C:\exported-data\1020_"</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -1023,15 +1033,15 @@
       </c>
       <c r="B38" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>Unity1021*.Value</v>
+        <v>Unit1021*.Value</v>
       </c>
       <c r="C38" t="str">
         <f t="shared" si="1"/>
-        <v>\\WYCVWAPPH186\D$\Stage\MDUS_Export\Reads\Extract_PH3_1021_</v>
+        <v>C:\exported-data\1021_</v>
       </c>
       <c r="D38" t="str">
         <f t="shared" si="2"/>
-        <v>DataReader.exe -s WYCWAPPH059 -t "Unity1021*.Value" --st " 23/07/2013 02:14:03" --et "16/05/2015 09:04:47" --estimatedEventsPerDay 1 --eventsPerRead 100000 --eventsPerFile 100000001 --estimatedTagscount 100000 --writersCount 8 --enableWrite --outFileName "\\WYCVWAPPH186\D$\Stage\MDUS_Export\Reads\Extract_PH3_1021_"</v>
+        <v>DataReader.exe -s PIDA01 -t "Unit1021*.Value" --st "2015-01-01 00:00:00" --et "2020-01-01 00:00:00" --estimatedEventsPerDay 1 --eventsPerRead 100000 --eventsPerFile 100000001 --estimatedTagscount 100000 --writersCount 8 --enableWrite --outFileName "C:\exported-data\1021_"</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -1040,15 +1050,15 @@
       </c>
       <c r="B39" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>Unity1022*.Value</v>
+        <v>Unit1022*.Value</v>
       </c>
       <c r="C39" t="str">
         <f t="shared" si="1"/>
-        <v>\\WYCVWAPPH186\D$\Stage\MDUS_Export\Reads\Extract_PH3_1022_</v>
+        <v>C:\exported-data\1022_</v>
       </c>
       <c r="D39" t="str">
         <f t="shared" si="2"/>
-        <v>DataReader.exe -s WYCWAPPH059 -t "Unity1022*.Value" --st " 23/07/2013 02:14:03" --et "16/05/2015 09:04:47" --estimatedEventsPerDay 1 --eventsPerRead 100000 --eventsPerFile 100000001 --estimatedTagscount 100000 --writersCount 8 --enableWrite --outFileName "\\WYCVWAPPH186\D$\Stage\MDUS_Export\Reads\Extract_PH3_1022_"</v>
+        <v>DataReader.exe -s PIDA01 -t "Unit1022*.Value" --st "2015-01-01 00:00:00" --et "2020-01-01 00:00:00" --estimatedEventsPerDay 1 --eventsPerRead 100000 --eventsPerFile 100000001 --estimatedTagscount 100000 --writersCount 8 --enableWrite --outFileName "C:\exported-data\1022_"</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -1057,15 +1067,15 @@
       </c>
       <c r="B40" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>Unity1023*.Value</v>
+        <v>Unit1023*.Value</v>
       </c>
       <c r="C40" t="str">
         <f t="shared" si="1"/>
-        <v>\\WYCVWAPPH186\D$\Stage\MDUS_Export\Reads\Extract_PH3_1023_</v>
+        <v>C:\exported-data\1023_</v>
       </c>
       <c r="D40" t="str">
         <f t="shared" si="2"/>
-        <v>DataReader.exe -s WYCWAPPH059 -t "Unity1023*.Value" --st " 23/07/2013 02:14:03" --et "16/05/2015 09:04:47" --estimatedEventsPerDay 1 --eventsPerRead 100000 --eventsPerFile 100000001 --estimatedTagscount 100000 --writersCount 8 --enableWrite --outFileName "\\WYCVWAPPH186\D$\Stage\MDUS_Export\Reads\Extract_PH3_1023_"</v>
+        <v>DataReader.exe -s PIDA01 -t "Unit1023*.Value" --st "2015-01-01 00:00:00" --et "2020-01-01 00:00:00" --estimatedEventsPerDay 1 --eventsPerRead 100000 --eventsPerFile 100000001 --estimatedTagscount 100000 --writersCount 8 --enableWrite --outFileName "C:\exported-data\1023_"</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -1074,15 +1084,15 @@
       </c>
       <c r="B41" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>Unity1024*.Value</v>
+        <v>Unit1024*.Value</v>
       </c>
       <c r="C41" t="str">
         <f t="shared" si="1"/>
-        <v>\\WYCVWAPPH186\D$\Stage\MDUS_Export\Reads\Extract_PH3_1024_</v>
+        <v>C:\exported-data\1024_</v>
       </c>
       <c r="D41" t="str">
         <f t="shared" si="2"/>
-        <v>DataReader.exe -s WYCWAPPH059 -t "Unity1024*.Value" --st " 23/07/2013 02:14:03" --et "16/05/2015 09:04:47" --estimatedEventsPerDay 1 --eventsPerRead 100000 --eventsPerFile 100000001 --estimatedTagscount 100000 --writersCount 8 --enableWrite --outFileName "\\WYCVWAPPH186\D$\Stage\MDUS_Export\Reads\Extract_PH3_1024_"</v>
+        <v>DataReader.exe -s PIDA01 -t "Unit1024*.Value" --st "2015-01-01 00:00:00" --et "2020-01-01 00:00:00" --estimatedEventsPerDay 1 --eventsPerRead 100000 --eventsPerFile 100000001 --estimatedTagscount 100000 --writersCount 8 --enableWrite --outFileName "C:\exported-data\1024_"</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -1091,15 +1101,15 @@
       </c>
       <c r="B42" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>Unity1025*.Value</v>
+        <v>Unit1025*.Value</v>
       </c>
       <c r="C42" t="str">
         <f t="shared" si="1"/>
-        <v>\\WYCVWAPPH186\D$\Stage\MDUS_Export\Reads\Extract_PH3_1025_</v>
+        <v>C:\exported-data\1025_</v>
       </c>
       <c r="D42" t="str">
         <f t="shared" si="2"/>
-        <v>DataReader.exe -s WYCWAPPH059 -t "Unity1025*.Value" --st " 23/07/2013 02:14:03" --et "16/05/2015 09:04:47" --estimatedEventsPerDay 1 --eventsPerRead 100000 --eventsPerFile 100000001 --estimatedTagscount 100000 --writersCount 8 --enableWrite --outFileName "\\WYCVWAPPH186\D$\Stage\MDUS_Export\Reads\Extract_PH3_1025_"</v>
+        <v>DataReader.exe -s PIDA01 -t "Unit1025*.Value" --st "2015-01-01 00:00:00" --et "2020-01-01 00:00:00" --estimatedEventsPerDay 1 --eventsPerRead 100000 --eventsPerFile 100000001 --estimatedTagscount 100000 --writersCount 8 --enableWrite --outFileName "C:\exported-data\1025_"</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -1108,18 +1118,19 @@
       </c>
       <c r="B43" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>Unity1026*.Value</v>
+        <v>Unit1026*.Value</v>
       </c>
       <c r="C43" t="str">
         <f t="shared" si="1"/>
-        <v>\\WYCVWAPPH186\D$\Stage\MDUS_Export\Reads\Extract_PH3_1026_</v>
+        <v>C:\exported-data\1026_</v>
       </c>
       <c r="D43" t="str">
         <f t="shared" si="2"/>
-        <v>DataReader.exe -s WYCWAPPH059 -t "Unity1026*.Value" --st " 23/07/2013 02:14:03" --et "16/05/2015 09:04:47" --estimatedEventsPerDay 1 --eventsPerRead 100000 --eventsPerFile 100000001 --estimatedTagscount 100000 --writersCount 8 --enableWrite --outFileName "\\WYCVWAPPH186\D$\Stage\MDUS_Export\Reads\Extract_PH3_1026_"</v>
+        <v>DataReader.exe -s PIDA01 -t "Unit1026*.Value" --st "2015-01-01 00:00:00" --et "2020-01-01 00:00:00" --estimatedEventsPerDay 1 --eventsPerRead 100000 --eventsPerFile 100000001 --estimatedTagscount 100000 --writersCount 8 --enableWrite --outFileName "C:\exported-data\1026_"</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>